<commit_message>
fixing merge problems in post and main
</commit_message>
<xml_diff>
--- a/src/main/java/com/selenium_project/resources/SignUpExcel/UsersInfoExcel.xlsx
+++ b/src/main/java/com/selenium_project/resources/SignUpExcel/UsersInfoExcel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Microsoft\Downloads\Selenium-QA-Project\src\main\java\com\selenium_project\resources\SignUpExcel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09BB7101-FC49-444C-A02C-79218A281942}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{683879FB-AB12-4D1B-9504-DF767BD60915}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{B74ECC32-4AE3-4E29-9748-769E5B66EB2A}"/>
   </bookViews>
@@ -143,10 +143,10 @@
     <t>bookmark_search</t>
   </si>
   <si>
-    <t>Ja</t>
-  </si>
-  <si>
     <t>os</t>
+  </si>
+  <si>
+    <t>Jane</t>
   </si>
 </sst>
 </file>
@@ -532,8 +532,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DBBF4BF-486D-4642-9F9C-97954569B52D}">
   <dimension ref="A1:Q3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="P2" sqref="P2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -647,10 +647,10 @@
         <v>32</v>
       </c>
       <c r="P2" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q2" t="s">
         <v>35</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.3">

</xml_diff>